<commit_message>
feat: new phoneCase options
</commit_message>
<xml_diff>
--- a/companies/trendyol/watchBand/WatchBand.xlsx
+++ b/companies/trendyol/watchBand/WatchBand.xlsx
@@ -224,7 +224,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -416,6 +416,16 @@
       <sz val="14.0"/>
       <b val="true"/>
       <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="8"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -565,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -745,7 +755,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="true"/>
     </xf>
@@ -770,6 +780,14 @@
       <protection locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="true"/>
     </xf>
@@ -1259,6 +1277,11 @@
           <t>Uyumlu Marka</t>
         </is>
       </c>
+      <c r="AC1" s="51" t="inlineStr">
+        <is>
+          <t>Uyumlu Model</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="D2" t="inlineStr">
@@ -1273,7 +1296,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="27">
+  <dataValidations count="28">
     <dataValidation type="list" sqref="Y2:Y1048576" allowBlank="true" errorStyle="stop" errorTitle="DEĞER SEÇİMİ HATASI" error="Sadece izin verilen değerleri girebilirsiniz. Lütfen kontrol ediniz." showErrorMessage="true">
       <formula1>Urun_Ozellik_Bilgileri!$A$2:$A$10</formula1>
     </dataValidation>
@@ -1286,14 +1309,17 @@
     <dataValidation type="list" sqref="AB2:AB1048576" allowBlank="true" errorStyle="stop" errorTitle="DEĞER SEÇİMİ HATASI" error="Sadece izin verilen değerleri girebilirsiniz. Lütfen kontrol ediniz." showErrorMessage="true">
       <formula1>Urun_Ozellik_Bilgileri!$D$2:$D$13</formula1>
     </dataValidation>
+    <dataValidation type="list" sqref="AC2:AC1048576" allowBlank="true" errorStyle="stop" errorTitle="DEĞER SEÇİMİ HATASI" error="Sadece izin verilen değerleri girebilirsiniz. Lütfen kontrol ediniz." showErrorMessage="true">
+      <formula1>Urun_Ozellik_Bilgileri!$E$2:$E$31</formula1>
+    </dataValidation>
     <dataValidation type="list" sqref="E2:E1048576" allowBlank="true" errorStyle="stop" promptTitle="PARA BİRİMİ GİRİN" prompt="Ürün fiyatının para birimi değerini girin." showInputMessage="true" errorTitle="DEĞER SEÇİMİ HATASI" error="Sadece izin verilen değerleri girebilirsiniz. Lütfen kontrol ediniz." showErrorMessage="true">
-      <formula1>Urun_Ozellik_Bilgileri!$E$2:$E$2</formula1>
+      <formula1>Urun_Ozellik_Bilgileri!$F$2:$F$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="L2:L1048576" allowBlank="true" errorStyle="stop" promptTitle="KDV ORANI GİRİN" prompt="KDV değerini listeden seçiniz." showInputMessage="true">
-      <formula1>Urun_Ozellik_Bilgileri!$F$2:$F$5</formula1>
+      <formula1>Urun_Ozellik_Bilgileri!$G$2:$G$5</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="W2:W1048576" allowBlank="true" errorStyle="stop" promptTitle="SEVKİYAT TİPİ GİRİN" prompt="Sevkiyat tipini listeden seçiniz." showInputMessage="true" errorTitle="DEĞER SEÇİMİ HATASI" error="Sadece izin verilen değerleri girebilirsiniz. Lütfen kontrol ediniz." showErrorMessage="true">
-      <formula1>Urun_Ozellik_Bilgileri!$G$2:$G$3</formula1>
+      <formula1>Urun_Ozellik_Bilgileri!$H$2:$H$3</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="between" sqref="V2:V1048576" allowBlank="true" errorStyle="stop" promptTitle="SEVKİYAT SÜRESİ GİRİN" prompt="Sadece sayı girebilirsiniz. ÖRNEK: 5" showInputMessage="true" errorTitle="SEVKİYAT SÜRESİ HATASI" error="Sevkiyat süresi değeri sadece sayı olmalıdır." showErrorMessage="true">
       <formula1>0</formula1>
@@ -1377,37 +1403,42 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="51" t="inlineStr">
+      <c r="A1" s="52" t="inlineStr">
         <is>
           <t>Beden</t>
         </is>
       </c>
-      <c r="B1" s="52" t="inlineStr">
+      <c r="B1" s="53" t="inlineStr">
         <is>
           <t>Garanti Süresi</t>
         </is>
       </c>
-      <c r="C1" s="53" t="inlineStr">
+      <c r="C1" s="54" t="inlineStr">
         <is>
           <t>Materyal</t>
         </is>
       </c>
-      <c r="D1" s="54" t="inlineStr">
+      <c r="D1" s="55" t="inlineStr">
         <is>
           <t>Uyumlu Marka</t>
         </is>
       </c>
-      <c r="E1" s="55" t="inlineStr">
+      <c r="E1" s="56" t="inlineStr">
+        <is>
+          <t>Uyumlu Model</t>
+        </is>
+      </c>
+      <c r="F1" s="57" t="inlineStr">
         <is>
           <t>Para Birimi</t>
         </is>
       </c>
-      <c r="F1" s="56" t="inlineStr">
+      <c r="G1" s="58" t="inlineStr">
         <is>
           <t>KDV Oranı</t>
         </is>
       </c>
-      <c r="G1" s="57" t="inlineStr">
+      <c r="H1" s="59" t="inlineStr">
         <is>
           <t>Sevkiyat Tipi</t>
         </is>
@@ -1436,15 +1467,20 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>Amazfit Band 7</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>TRY</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Hızlı Teslimat</t>
         </is>
@@ -1471,12 +1507,17 @@
           <t>Apple</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Amazfit GTR</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Bugün Kargoda</t>
         </is>
@@ -1503,7 +1544,12 @@
           <t>Belirtilmemiş</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Amazfit GTS</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -1530,7 +1576,12 @@
           <t>Fitbit</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Amazfit Pace</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>20</t>
         </is>
@@ -1557,6 +1608,11 @@
           <t>Garmin</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Apple Watch</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1579,6 +1635,11 @@
           <t>Haylou</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Apple Watch Ultra</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1601,6 +1662,11 @@
           <t>Honor</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Belirtilmemiş</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1613,6 +1679,11 @@
           <t>Huawei</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Galaxy Watch</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1625,6 +1696,11 @@
           <t>Oppo</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Haylou Solar LS05</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="D11" t="inlineStr">
@@ -1632,6 +1708,11 @@
           <t>Samsung</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Huawei Band 6</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="D12" t="inlineStr">
@@ -1639,11 +1720,147 @@
           <t>Winex</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Huawei Band 7</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="D13" t="inlineStr">
         <is>
           <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Huawei Band 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Huawei Honor Magic 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Huawei Watch 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Huawei Watch 3 Pro</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Huawei Watch 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Huawei Watch 4 Pro</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Huawei Watch Fit</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Huawei Watch GT2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Huawei Watch GT2 Pro</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Huawei Watch GT3</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Huawei Watch GT3 Pro</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Huawei Watch GT4</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Mi Watch Color</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Mi Watch Lite 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Oppo Watch</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Redmi Smart Band 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Redmi Watch 2 Lite</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Redmi Watch 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Redmi Watch 3 Active</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: screenProtector & updated outdated trendyol fields
</commit_message>
<xml_diff>
--- a/companies/trendyol/watchBand/WatchBand.xlsx
+++ b/companies/trendyol/watchBand/WatchBand.xlsx
@@ -1462,7 +1462,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Amazfit</t>
+          <t>Amazfit Uyumlu</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1504,7 +1504,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>Apple Uyumlu</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Fitbit</t>
+          <t>Fitbit Uyumlu</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Garmin</t>
+          <t>Garmin Uyumlu</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Haylou</t>
+          <t>Haylou Uyumlu</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Honor</t>
+          <t>Honor Uyumlu</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Huawei</t>
+          <t>Huawei Uyumlu</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Oppo</t>
+          <t>Oppo Uyumlu</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1705,7 +1705,7 @@
     <row r="11">
       <c r="D11" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Samsung Uyumlu</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1717,7 +1717,7 @@
     <row r="12">
       <c r="D12" t="inlineStr">
         <is>
-          <t>Winex</t>
+          <t>Winex Uyumlu</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1729,7 +1729,7 @@
     <row r="13">
       <c r="D13" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Xiaomi Uyumlu</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">

</xml_diff>